<commit_message>
continued editing of v01. Added error message for incorrect inputs
</commit_message>
<xml_diff>
--- a/Bloom Charts.xlsx
+++ b/Bloom Charts.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
@@ -935,12 +935,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>99</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -950,7 +950,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Hit</t>
+          <t>Strike looking</t>
         </is>
       </c>
     </row>
@@ -967,22 +967,22 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>88</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>FB</t>
+          <t>SL</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Strike looking</t>
+          <t>Foul Ball</t>
         </is>
       </c>
     </row>
@@ -999,12 +999,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>99</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1014,93 +1014,93 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Ball</t>
+          <t>Strikeout looking</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Joe</t>
+          <t>Woody</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/20/2023</t>
+          <t>03/30/2023</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>98</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>SL</t>
+          <t>FB</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Foul Ball</t>
+          <t>Strike looking</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Joe</t>
+          <t>Andrew Armstrong</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/20/2023</t>
+          <t>09/23/2023</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>98</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Knuck</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Hit</t>
+          <t>Strike looking</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Joe</t>
+          <t>Andrew Armstrong</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/20/2023</t>
+          <t>09/22/2023</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>23</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1110,71 +1110,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Strikeout looking</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Joe</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>4/20/2023</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>FB</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Strikeout swinging</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Woody</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>03/30/2023</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>FB</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Strike looking</t>
+          <t>Strike swing &amp; miss</t>
         </is>
       </c>
     </row>
@@ -1189,7 +1125,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A16" sqref="A16:XFD16"/>
@@ -1918,12 +1854,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>99</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1933,7 +1869,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Hit</t>
+          <t>Strike looking</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1943,12 +1879,12 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Swing contact</t>
+          <t>No swing</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>not free base</t>
+          <t>nothing</t>
         </is>
       </c>
     </row>
@@ -1965,22 +1901,22 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>88</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>FB</t>
+          <t>SL</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Strike looking</t>
+          <t>Foul Ball</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1990,7 +1926,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>No swing</t>
+          <t>Swing contact</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -2012,12 +1948,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>99</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -2027,12 +1963,12 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Ball</t>
+          <t>Strikeout looking</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Ball</t>
+          <t>Strike</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -2042,39 +1978,39 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>nothing</t>
+          <t>not free base</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Joe</t>
+          <t>Woody</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/20/2023</t>
+          <t>03/30/2023</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>98</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>SL</t>
+          <t>FB</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Foul Ball</t>
+          <t>Strike looking</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -2084,7 +2020,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Swing contact</t>
+          <t>No swing</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -2096,32 +2032,32 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Joe</t>
+          <t>Andrew Armstrong</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/20/2023</t>
+          <t>09/23/2023</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>98</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Knuck</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Hit</t>
+          <t>Strike looking</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -2131,34 +2067,34 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Swing contact</t>
+          <t>No swing</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>not free base</t>
+          <t>nothing</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Joe</t>
+          <t>Andrew Armstrong</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/20/2023</t>
+          <t>09/22/2023</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>23</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -2168,7 +2104,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Strikeout looking</t>
+          <t>Strike swing &amp; miss</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -2178,104 +2114,10 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>No swing</t>
+          <t>Swing no contact</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
-        <is>
-          <t>not free base</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Joe</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>4/20/2023</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>FB</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Strikeout swinging</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Strike</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Swing no contact</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>not free base</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Woody</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>03/30/2023</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>FB</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Strike looking</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Strike</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>No swing</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
         <is>
           <t>nothing</t>
         </is>
@@ -2292,7 +2134,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
@@ -2452,27 +2294,58 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>96.8</v>
+        <v>99</v>
       </c>
       <c r="C5" t="n">
         <v>99</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>23</v>
+      </c>
+      <c r="C6" t="n">
+        <v>23</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more fixes for error messages
</commit_message>
<xml_diff>
--- a/Bloom Charts.xlsx
+++ b/Bloom Charts.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
@@ -482,34 +482,158 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>09/22/2023</t>
+          <t>09/23/2023</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Foul Ball</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="18.75" customHeight="1" s="1">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>FB</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Strikeout looking</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="18.75" customHeight="1" s="1"/>
-    <row r="4" ht="18.75" customHeight="1" s="1"/>
-    <row r="5" ht="18.75" customHeight="1" s="1"/>
-    <row r="6" ht="18.75" customHeight="1" s="1"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Strike looking</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="18.75" customHeight="1" s="1">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Hit</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="18.75" customHeight="1" s="1">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>SL</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Strike looking</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="18.75" customHeight="1" s="1">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>SL</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Strike swing &amp; miss</t>
+        </is>
+      </c>
+    </row>
     <row r="7" ht="18.75" customHeight="1" s="1"/>
     <row r="8" ht="18.75" customHeight="1" s="1"/>
     <row r="9" ht="18.75" customHeight="1" s="1"/>
@@ -531,7 +655,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A16" sqref="A16:XFD16"/>
@@ -597,7 +721,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>09/22/2023</t>
+          <t>09/23/2023</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -617,29 +741,213 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>Foul Ball</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Strike</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Swing contact</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nothing</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="18.75" customHeight="1" s="1">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>Strike looking</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Strike</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>No swing</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>nothing</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="18.75" customHeight="1" s="1"/>
-    <row r="4" ht="18.75" customHeight="1" s="1"/>
-    <row r="5" ht="18.75" customHeight="1" s="1"/>
-    <row r="6" ht="18.75" customHeight="1" s="1"/>
+    <row r="4" ht="18.75" customHeight="1" s="1">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Hit</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Strike</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Swing contact</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>not free base</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="18.75" customHeight="1" s="1">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>SL</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Strike looking</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Strike</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>No swing</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nothing</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="18.75" customHeight="1" s="1">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>SL</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Strike swing &amp; miss</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Strike</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Swing no contact</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nothing</t>
+        </is>
+      </c>
+    </row>
     <row r="7" ht="18.75" customHeight="1" s="1"/>
     <row r="8" ht="18.75" customHeight="1" s="1"/>
     <row r="9" ht="18.75" customHeight="1" s="1"/>
@@ -727,25 +1035,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>90</v>
+        <v>89.7</v>
       </c>
       <c r="C2" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H2" t="n">
         <v>1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Made it so that treeview will always default to see the most recent input
</commit_message>
<xml_diff>
--- a/Bloom Charts.xlsx
+++ b/Bloom Charts.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
@@ -634,16 +634,390 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="18.75" customHeight="1" s="1"/>
-    <row r="8" ht="18.75" customHeight="1" s="1"/>
-    <row r="9" ht="18.75" customHeight="1" s="1"/>
-    <row r="10" ht="18.75" customHeight="1" s="1"/>
-    <row r="11" ht="18.75" customHeight="1" s="1"/>
-    <row r="12" ht="18.75" customHeight="1" s="1"/>
-    <row r="13" ht="18.75" customHeight="1" s="1"/>
-    <row r="14" ht="18.75" customHeight="1" s="1"/>
-    <row r="15" ht="18.75" customHeight="1" s="1"/>
-    <row r="16" ht="18.75" customHeight="1" s="1"/>
+    <row r="7" ht="18.75" customHeight="1" s="1">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>CH</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="18.75" customHeight="1" s="1">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>SL</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>HBP</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="18.75" customHeight="1" s="1">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Strike looking</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="18.75" customHeight="1" s="1">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Foul Ball</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="18.75" customHeight="1" s="1">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="18.75" customHeight="1" s="1">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>CB</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="18.75" customHeight="1" s="1">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Strikeout swinging</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="18.75" customHeight="1" s="1">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Hit</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="18.75" customHeight="1" s="1">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Knuck</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="18.75" customHeight="1" s="1">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Knuck</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Walk</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -655,7 +1029,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A16" sqref="A16:XFD16"/>
@@ -948,15 +1322,570 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="18.75" customHeight="1" s="1"/>
-    <row r="8" ht="18.75" customHeight="1" s="1"/>
-    <row r="9" ht="18.75" customHeight="1" s="1"/>
-    <row r="10" ht="18.75" customHeight="1" s="1"/>
-    <row r="11" ht="18.75" customHeight="1" s="1"/>
-    <row r="12" ht="18.75" customHeight="1" s="1"/>
-    <row r="13" ht="18.75" customHeight="1" s="1"/>
-    <row r="14" ht="18.75" customHeight="1" s="1"/>
-    <row r="15" ht="18.75" customHeight="1" s="1"/>
+    <row r="7" ht="18.75" customHeight="1" s="1">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>CH</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>No swing</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nothing</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="18.75" customHeight="1" s="1">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>SL</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>HBP</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>No swing</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>free base</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="18.75" customHeight="1" s="1">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Strike looking</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Strike</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>No swing</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nothing</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="18.75" customHeight="1" s="1">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Foul Ball</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Strike</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Swing contact</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nothing</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="18.75" customHeight="1" s="1">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>No swing</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nothing</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="18.75" customHeight="1" s="1">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>CB</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>No swing</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nothing</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="18.75" customHeight="1" s="1">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Strikeout swinging</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Strike</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Swing no contact</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>not free base</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="18.75" customHeight="1" s="1">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Hit</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Strike</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Swing contact</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>not free base</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="18.75" customHeight="1" s="1">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Knuck</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>No swing</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>nothing</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>No swing</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>nothing</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>No swing</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>nothing</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Knuck</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Walk</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>No swing</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>free base</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1038,25 +1967,25 @@
         <v>89.7</v>
       </c>
       <c r="C2" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E2" t="n">
         <v>0.3</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="G2" t="n">
         <v>0.3</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" ht="18.75" customHeight="1" s="1"/>

</xml_diff>

<commit_message>
Got the ab tracker
</commit_message>
<xml_diff>
--- a/Bloom Charts.xlsx
+++ b/Bloom Charts.xlsx
@@ -3,30 +3,34 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="pitch breakdown" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="pitcher breakdown" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'pitcher breakdown'!$A$1:$F$1</definedName>
-  </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -56,9 +60,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
@@ -143,10 +161,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -184,71 +202,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -276,7 +294,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -299,11 +317,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -312,13 +330,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -328,7 +346,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -337,7 +355,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -346,7 +364,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -354,10 +372,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -429,686 +447,687 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.54296875" bestFit="1" customWidth="1" style="1" min="1" max="2"/>
-    <col width="12" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
-    <col width="13.54296875" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
-    <col width="9.26953125" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
-    <col width="13.54296875" bestFit="1" customWidth="1" style="1" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
+    <col width="12.005" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="9.290714285714287" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Pitcher</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Pitch Counter</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Velo</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>Pitch Type</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>Result</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="18.75" customHeight="1" s="1">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Andrew Armstrong</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="5" t="inlineStr">
         <is>
           <t>90</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="5" t="inlineStr">
         <is>
           <t>FB</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="5" t="inlineStr">
         <is>
           <t>Foul Ball</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="18.75" customHeight="1" s="1">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Andrew Armstrong</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="5" t="inlineStr">
         <is>
           <t>91</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="5" t="inlineStr">
         <is>
           <t>FB</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="5" t="inlineStr">
         <is>
           <t>Strike looking</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="18.75" customHeight="1" s="1">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Andrew Armstrong</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="5" t="inlineStr">
         <is>
           <t>88</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="5" t="inlineStr">
         <is>
           <t>FB</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="5" t="inlineStr">
         <is>
           <t>Hit</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="18.75" customHeight="1" s="1">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Andrew Armstrong</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
+    <row r="5" ht="18.75" customHeight="1">
+      <c r="A5" s="5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="5" t="inlineStr">
         <is>
           <t>88</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" s="5" t="inlineStr">
         <is>
           <t>SL</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="5" t="inlineStr">
         <is>
           <t>Strike looking</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="18.75" customHeight="1" s="1">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Andrew Armstrong</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
+    <row r="6" ht="18.75" customHeight="1">
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="5" t="inlineStr">
         <is>
           <t>85</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" s="5" t="inlineStr">
         <is>
           <t>SL</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" s="5" t="inlineStr">
         <is>
           <t>Strike swing &amp; miss</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="18.75" customHeight="1" s="1">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Andrew Armstrong</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
+    <row r="7" ht="18.75" customHeight="1">
+      <c r="A7" s="5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="5" t="inlineStr">
         <is>
           <t>84</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" s="5" t="inlineStr">
         <is>
           <t>CH</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Ball</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="18.75" customHeight="1" s="1">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Andrew Armstrong</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
+    <row r="8" ht="18.75" customHeight="1">
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B8" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="5" t="inlineStr">
         <is>
           <t>88</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" s="5" t="inlineStr">
         <is>
           <t>SL</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" s="5" t="inlineStr">
         <is>
           <t>HBP</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="18.75" customHeight="1" s="1">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Andrew Armstrong</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
+    <row r="9" ht="18.75" customHeight="1">
+      <c r="A9" s="5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C9" s="5" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="5" t="inlineStr">
         <is>
           <t>90</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" s="5" t="inlineStr">
         <is>
           <t>FB</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" s="5" t="inlineStr">
         <is>
           <t>Strike looking</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="18.75" customHeight="1" s="1">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Andrew Armstrong</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
+    <row r="10" ht="18.75" customHeight="1">
+      <c r="A10" s="5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="5" t="inlineStr">
         <is>
           <t>92</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" s="5" t="inlineStr">
         <is>
           <t>FB</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" s="5" t="inlineStr">
         <is>
           <t>Foul Ball</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="18.75" customHeight="1" s="1">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Andrew Armstrong</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
+    <row r="11" ht="18.75" customHeight="1">
+      <c r="A11" s="5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B11" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C11" s="5" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="5" t="inlineStr">
         <is>
           <t>90</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E11" s="5" t="inlineStr">
         <is>
           <t>FB</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" s="5" t="inlineStr">
         <is>
           <t>Ball</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="18.75" customHeight="1" s="1">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Andrew Armstrong</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
+    <row r="12" ht="18.75" customHeight="1">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="5" t="inlineStr">
         <is>
           <t>77</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E12" s="5" t="inlineStr">
         <is>
           <t>CB</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" s="5" t="inlineStr">
         <is>
           <t>Ball</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="18.75" customHeight="1" s="1">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Andrew Armstrong</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
+    <row r="13" ht="18.75" customHeight="1">
+      <c r="A13" s="5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="5" t="inlineStr">
         <is>
           <t>88</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E13" s="5" t="inlineStr">
         <is>
           <t>FB</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" s="5" t="inlineStr">
         <is>
           <t>Strikeout swinging</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="18.75" customHeight="1" s="1">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Andrew Armstrong</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
+    <row r="14" ht="18.75" customHeight="1">
+      <c r="A14" s="5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
         <is>
           <t>13</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="5" t="inlineStr">
         <is>
           <t>90</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E14" s="5" t="inlineStr">
         <is>
           <t>FB</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" s="5" t="inlineStr">
         <is>
           <t>Hit</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="18.75" customHeight="1" s="1">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Andrew Armstrong</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
+    <row r="15" ht="18.75" customHeight="1">
+      <c r="A15" s="5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
         <is>
           <t>14</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" s="5" t="inlineStr">
         <is>
           <t>88</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E15" s="5" t="inlineStr">
         <is>
           <t>Knuck</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F15" s="5" t="inlineStr">
         <is>
           <t>Ball</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="18.75" customHeight="1" s="1">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Andrew Armstrong</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
+    <row r="16" ht="18.75" customHeight="1">
+      <c r="A16" s="5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B16" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C16" s="5" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D16" s="5" t="inlineStr">
         <is>
           <t>90</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E16" s="5" t="inlineStr">
         <is>
           <t>FB</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F16" s="5" t="inlineStr">
         <is>
           <t>Ball</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Andrew Armstrong</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
+    <row r="17" ht="18.75" customHeight="1">
+      <c r="A17" s="5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D17" s="5" t="inlineStr">
         <is>
           <t>88</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E17" s="5" t="inlineStr">
         <is>
           <t>FB</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F17" s="5" t="inlineStr">
         <is>
           <t>Ball</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Andrew Armstrong</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
+    <row r="18" ht="18.75" customHeight="1">
+      <c r="A18" s="5" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
         <is>
           <t>17</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D18" s="5" t="inlineStr">
         <is>
           <t>75</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="E18" s="5" t="inlineStr">
         <is>
           <t>Knuck</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F18" s="5" t="inlineStr">
         <is>
           <t>Walk</t>
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
+    <row r="19" ht="18.75" customHeight="1">
+      <c r="A19" s="5" t="inlineStr">
         <is>
           <t>Nate Baranski</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
+      <c r="B19" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C19" s="5" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="D19" s="5" t="inlineStr">
         <is>
           <t>90</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="E19" s="5" t="inlineStr">
         <is>
           <t>FB</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="F19" s="5" t="inlineStr">
         <is>
           <t>Strike looking</t>
         </is>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
+    <row r="20" ht="18.75" customHeight="1">
+      <c r="A20" s="5" t="inlineStr">
         <is>
           <t>Nate Baranski</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
+      <c r="B20" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C20" s="5" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D20" s="5" t="inlineStr">
         <is>
           <t>92</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E20" s="5" t="inlineStr">
         <is>
           <t>FB</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="F20" s="5" t="inlineStr">
         <is>
           <t>Strike looking</t>
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
+    <row r="21" ht="18.75" customHeight="1">
+      <c r="A21" s="5" t="inlineStr">
         <is>
           <t>Nate Baranski</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>09/23/2023</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
+      <c r="B21" s="5" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C21" s="5" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="D21" s="5" t="inlineStr">
         <is>
           <t>94</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="E21" s="5" t="inlineStr">
         <is>
           <t>FB</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="F21" s="5" t="inlineStr">
         <is>
           <t>Strikeout swinging</t>
         </is>
@@ -1125,65 +1144,85 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.54296875" bestFit="1" customWidth="1" style="1" min="1" max="9"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="8" max="8"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="9" max="9"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="10" max="10"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="11" max="11"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Pitcher</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Pitch Counter</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Velo</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>Pitch Type</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>Result</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>Strike or Ball</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="5" t="inlineStr">
         <is>
           <t>Swing</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>Free Bases</t>
         </is>
       </c>
-    </row>
-    <row r="2" ht="18.75" customHeight="1" s="1">
+      <c r="J1" s="5" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="K1" s="5" t="inlineStr">
+        <is>
+          <t>ab</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="18.75" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
           <t>Andrew Armstrong</t>
@@ -1229,8 +1268,18 @@
           <t>nothing</t>
         </is>
       </c>
-    </row>
-    <row r="3" ht="18.75" customHeight="1" s="1">
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>not event</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>new ab 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="18.75" customHeight="1">
       <c r="A3" t="inlineStr">
         <is>
           <t>Andrew Armstrong</t>
@@ -1276,8 +1325,18 @@
           <t>nothing</t>
         </is>
       </c>
-    </row>
-    <row r="4" ht="18.75" customHeight="1" s="1">
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>not event</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>new ab 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="18.75" customHeight="1">
       <c r="A4" t="inlineStr">
         <is>
           <t>Andrew Armstrong</t>
@@ -1323,8 +1382,18 @@
           <t>not free base</t>
         </is>
       </c>
-    </row>
-    <row r="5" ht="18.75" customHeight="1" s="1">
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>event</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>new ab 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="18.75" customHeight="1">
       <c r="A5" t="inlineStr">
         <is>
           <t>Andrew Armstrong</t>
@@ -1370,8 +1439,18 @@
           <t>nothing</t>
         </is>
       </c>
-    </row>
-    <row r="6" ht="18.75" customHeight="1" s="1">
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>not event</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>new ab 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="18.75" customHeight="1">
       <c r="A6" t="inlineStr">
         <is>
           <t>Andrew Armstrong</t>
@@ -1417,8 +1496,18 @@
           <t>nothing</t>
         </is>
       </c>
-    </row>
-    <row r="7" ht="18.75" customHeight="1" s="1">
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>not event</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>new ab 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="18.75" customHeight="1">
       <c r="A7" t="inlineStr">
         <is>
           <t>Andrew Armstrong</t>
@@ -1464,8 +1553,18 @@
           <t>nothing</t>
         </is>
       </c>
-    </row>
-    <row r="8" ht="18.75" customHeight="1" s="1">
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>not event</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>new ab 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="18.75" customHeight="1">
       <c r="A8" t="inlineStr">
         <is>
           <t>Andrew Armstrong</t>
@@ -1511,8 +1610,18 @@
           <t>free base</t>
         </is>
       </c>
-    </row>
-    <row r="9" ht="18.75" customHeight="1" s="1">
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>event</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>new ab 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="18.75" customHeight="1">
       <c r="A9" t="inlineStr">
         <is>
           <t>Andrew Armstrong</t>
@@ -1558,8 +1667,18 @@
           <t>nothing</t>
         </is>
       </c>
-    </row>
-    <row r="10" ht="18.75" customHeight="1" s="1">
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>not event</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>new ab 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="18.75" customHeight="1">
       <c r="A10" t="inlineStr">
         <is>
           <t>Andrew Armstrong</t>
@@ -1605,8 +1724,18 @@
           <t>nothing</t>
         </is>
       </c>
-    </row>
-    <row r="11" ht="18.75" customHeight="1" s="1">
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>not event</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>new ab 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="18.75" customHeight="1">
       <c r="A11" t="inlineStr">
         <is>
           <t>Andrew Armstrong</t>
@@ -1652,8 +1781,18 @@
           <t>nothing</t>
         </is>
       </c>
-    </row>
-    <row r="12" ht="18.75" customHeight="1" s="1">
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>not event</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>new ab 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="18.75" customHeight="1">
       <c r="A12" t="inlineStr">
         <is>
           <t>Andrew Armstrong</t>
@@ -1699,8 +1838,18 @@
           <t>nothing</t>
         </is>
       </c>
-    </row>
-    <row r="13" ht="18.75" customHeight="1" s="1">
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>not event</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>new ab 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="18.75" customHeight="1">
       <c r="A13" t="inlineStr">
         <is>
           <t>Andrew Armstrong</t>
@@ -1746,8 +1895,18 @@
           <t>not free base</t>
         </is>
       </c>
-    </row>
-    <row r="14" ht="18.75" customHeight="1" s="1">
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>event</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>new ab 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="18.75" customHeight="1">
       <c r="A14" t="inlineStr">
         <is>
           <t>Andrew Armstrong</t>
@@ -1793,8 +1952,18 @@
           <t>not free base</t>
         </is>
       </c>
-    </row>
-    <row r="15" ht="18.75" customHeight="1" s="1">
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>event</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>new ab 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="18.75" customHeight="1">
       <c r="A15" t="inlineStr">
         <is>
           <t>Andrew Armstrong</t>
@@ -1840,8 +2009,18 @@
           <t>nothing</t>
         </is>
       </c>
-    </row>
-    <row r="16">
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>not event</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>new ab 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="18.75" customHeight="1">
       <c r="A16" t="inlineStr">
         <is>
           <t>Andrew Armstrong</t>
@@ -1887,8 +2066,18 @@
           <t>nothing</t>
         </is>
       </c>
-    </row>
-    <row r="17">
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>not event</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>new ab 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="18.75" customHeight="1">
       <c r="A17" t="inlineStr">
         <is>
           <t>Andrew Armstrong</t>
@@ -1934,8 +2123,18 @@
           <t>nothing</t>
         </is>
       </c>
-    </row>
-    <row r="18">
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>not event</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>new ab 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="18.75" customHeight="1">
       <c r="A18" t="inlineStr">
         <is>
           <t>Andrew Armstrong</t>
@@ -1981,8 +2180,18 @@
           <t>free base</t>
         </is>
       </c>
-    </row>
-    <row r="19">
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>event</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>new ab 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="18.75" customHeight="1">
       <c r="A19" t="inlineStr">
         <is>
           <t>Nate Baranski</t>
@@ -2028,8 +2237,18 @@
           <t>nothing</t>
         </is>
       </c>
-    </row>
-    <row r="20">
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>not event</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>new ab 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="18.75" customHeight="1">
       <c r="A20" t="inlineStr">
         <is>
           <t>Nate Baranski</t>
@@ -2075,8 +2294,18 @@
           <t>nothing</t>
         </is>
       </c>
-    </row>
-    <row r="21">
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>not event</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>new ab 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="18.75" customHeight="1">
       <c r="A21" t="inlineStr">
         <is>
           <t>Nate Baranski</t>
@@ -2120,6 +2349,16 @@
       <c r="I21" t="inlineStr">
         <is>
           <t>not free base</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>event</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>new ab 5</t>
         </is>
       </c>
     </row>
@@ -2134,110 +2373,166 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.54296875" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
-    <col width="13.54296875" bestFit="1" customWidth="1" style="2" min="2" max="3"/>
-    <col width="13.54296875" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="8" max="8"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="9" max="9"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Pitcher</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>avg FB</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Top FB</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>Strike %</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="6" t="inlineStr">
+        <is>
+          <t>Whiff %</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
         <is>
           <t>CSW %</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" s="6" t="inlineStr">
+        <is>
+          <t>FB CSW %</t>
+        </is>
+      </c>
+      <c r="H1" s="6" t="inlineStr">
+        <is>
+          <t>OffSpeed CSW %</t>
+        </is>
+      </c>
+      <c r="I1" s="6" t="inlineStr">
         <is>
           <t>Free Bases</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="18.75" customHeight="1" s="1">
+    <row r="2" ht="18.75" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Andrew Armstrong</t>
+          <t>Pitcher</t>
         </is>
       </c>
       <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Andrew Armstrong</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>89.7</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C3" t="n">
         <v>92</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>52.9%</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>33.3%</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
+      <c r="D3" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="I3" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="3" ht="18.75" customHeight="1" s="1">
-      <c r="A3" t="inlineStr">
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Nate Baranski</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B4" t="n">
         <v>92</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C4" t="n">
         <v>94</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" ht="18.75" customHeight="1" s="1"/>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F1">
-    <sortState ref="A2:F5">
-      <sortCondition descending="1" ref="D1"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ran exe file for version 0.1 and continued working on Pitch count tracking
</commit_message>
<xml_diff>
--- a/Bloom Charts.xlsx
+++ b/Bloom Charts.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1133,6 +1133,70 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Nate Baranski</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>CH</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Nate Baranski</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>CH</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>HBP</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1144,7 +1208,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1275,7 +1339,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>new ab 1</t>
+          <t>ab 1</t>
         </is>
       </c>
     </row>
@@ -1332,7 +1396,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>new ab 1</t>
+          <t>ab 1</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1453,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>new ab 1</t>
+          <t>ab 1</t>
         </is>
       </c>
     </row>
@@ -1446,7 +1510,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>new ab 2</t>
+          <t>ab 2</t>
         </is>
       </c>
     </row>
@@ -1503,7 +1567,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>new ab 2</t>
+          <t>ab 2</t>
         </is>
       </c>
     </row>
@@ -1560,7 +1624,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>new ab 2</t>
+          <t>ab 2</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1681,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>new ab 2</t>
+          <t>ab 2</t>
         </is>
       </c>
     </row>
@@ -1674,7 +1738,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>new ab 3</t>
+          <t>ab 3</t>
         </is>
       </c>
     </row>
@@ -1731,7 +1795,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>new ab 3</t>
+          <t>ab 3</t>
         </is>
       </c>
     </row>
@@ -1788,7 +1852,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>new ab 3</t>
+          <t>ab 3</t>
         </is>
       </c>
     </row>
@@ -1845,7 +1909,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>new ab 3</t>
+          <t>ab 3</t>
         </is>
       </c>
     </row>
@@ -1902,7 +1966,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>new ab 3</t>
+          <t>ab 3</t>
         </is>
       </c>
     </row>
@@ -1959,7 +2023,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>new ab 3</t>
+          <t>ab 4</t>
         </is>
       </c>
     </row>
@@ -2016,7 +2080,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>new ab 4</t>
+          <t>ab 5</t>
         </is>
       </c>
     </row>
@@ -2073,7 +2137,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>new ab 4</t>
+          <t>ab 5</t>
         </is>
       </c>
     </row>
@@ -2130,7 +2194,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>new ab 4</t>
+          <t>ab 5</t>
         </is>
       </c>
     </row>
@@ -2187,7 +2251,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>new ab 4</t>
+          <t>ab 5</t>
         </is>
       </c>
     </row>
@@ -2244,7 +2308,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>new ab 5</t>
+          <t>ab 6</t>
         </is>
       </c>
     </row>
@@ -2301,7 +2365,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>new ab 5</t>
+          <t>ab 6</t>
         </is>
       </c>
     </row>
@@ -2358,7 +2422,121 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>new ab 5</t>
+          <t>ab 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Nate Baranski</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>CH</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>No swing</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>nothing</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>not event</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>ab 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Nate Baranski</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>09/23/2023</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>CH</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>HBP</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>No swing</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>free base</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>event</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>ab 7</t>
         </is>
       </c>
     </row>
@@ -2514,13 +2692,13 @@
         <v>94</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -2529,7 +2707,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>